<commit_message>
added db and fetch licenses function
</commit_message>
<xml_diff>
--- a/my_excel_file_user_auth.xlsx
+++ b/my_excel_file_user_auth.xlsx
@@ -494,7 +494,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1:E1"/>
@@ -532,130 +532,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1e63519a-3baa-4299-bf06-b91402903c1d</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Francesco Pisani</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>f.pisani@pseudonymph.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>d9384421-525c-4e3f-9256-01c19745c0b0</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Roberto Sannazzaro</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>r.sannazzaro@pseudonymph.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>cb20b436-3933-4009-b704-56d254d24146</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>On-Premises Directory Synchronization Service Account</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Sync_WIN-LF0GIVMIMJI_2399cdb4f0a3@tommasoungettioutlook.onmicrosoft.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>36239a8b-d1f7-4ab5-b8bb-b770c6907505</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Tommaso Maria Ungetti</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Fucktotum</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>t.ungetti@pseudonymph.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>0b382b87-20c0-47e7-b6ed-d090bd85bcd6</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Tommaso Maria Ungetti</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>t.ungetti4047@tommasoungettioutlook.onmicrosoft.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>371d0525-ec47-4294-a1ea-9f337144f9c5</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Tommaso Maria Ungetti</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>tommaso.ungetti_outlook.com#EXT#@tommasoungettioutlook.onmicrosoft.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>43a29c46-0789-4425-b4cd-b9c87e4df6b9</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Valeria Marotta</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>v.marotta@pseudonymph.com</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -667,7 +543,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
@@ -701,303 +577,6 @@
           <t>Members</t>
         </is>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>12f6cf1c-f52e-4c77-afd3-081a2f47bc06</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>ADSyncOperators</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>ADSyncOperators</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>pseudonymph.com</t>
-        </is>
-      </c>
-      <c r="E2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>3bc7d838-fd96-4b6e-993c-323c0d8df7c2</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>SQLServer2005SQLBrowserUser$WIN-LF0GIVMIMJI</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Members in the group have the required access and privileges to be assigned as the log on account for the associated instance of SQL Server Browser.</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>pseudonymph.com</t>
-        </is>
-      </c>
-      <c r="E3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>44ab11dd-7311-44ba-b48f-e84356991995</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>ADSyncAdmins</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>ADSyncAdmins</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>pseudonymph.com</t>
-        </is>
-      </c>
-      <c r="E4" t="b">
-        <v>1</v>
-      </c>
-      <c r="F4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>463dead8-e8ef-4067-becf-ab94aff5ef23</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>ADSyncPasswordSet</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>ADSyncPasswordSet</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>pseudonymph.com</t>
-        </is>
-      </c>
-      <c r="E5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>47e009df-3599-4e89-8bf4-ad821c85c07f</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>ADSyncBrowse</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>ADSyncBrowse</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>pseudonymph.com</t>
-        </is>
-      </c>
-      <c r="E6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>528828d1-61a7-41c0-ba22-304a71f1b245</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>DnsUpdateProxy</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>DNS clients who are permitted to perform dynamic updates on behalf of some other clients (such as DHCP servers).</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>pseudonymph.com</t>
-        </is>
-      </c>
-      <c r="E7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>5fc95fad-3fe4-45ea-9a6a-8ca7393aadff</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>PROVA</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Tommaso Maria Ungetti, Roberto Sannazzaro, Valeria Marotta, Francesco Pisani, Tommaso Maria Ungetti</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>6130ca42-cae0-4c07-bd69-16638c5f2643</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>DnsAdmins</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>DNS Administrators Group</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>pseudonymph.com</t>
-        </is>
-      </c>
-      <c r="E9" t="b">
-        <v>1</v>
-      </c>
-      <c r="F9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>7266398f-bfe4-40b1-afe2-48e15c145be3</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>SQLRUserGroupHERMES01</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>SQLRUserGroupHERMES01</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>pseudonymph.com</t>
-        </is>
-      </c>
-      <c r="E10" t="b">
-        <v>1</v>
-      </c>
-      <c r="F10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>a1af16c5-26cb-41bd-bae7-68d20a02bb38</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>TeamTCMS</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>pseudonymph.com</t>
-        </is>
-      </c>
-      <c r="E11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>c2a3b6e5-985f-4df5-a080-8d092888cf6a</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>SQLServerMSASUser$WIN-LF0GIVMIMJI$HERMES01</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Members in the group have the required access and privileges to be assigned as the logon account for the associated instance of SQL Server 2019 Analysis Services.</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>pseudonymph.com</t>
-        </is>
-      </c>
-      <c r="E12" t="b">
-        <v>1</v>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>Tommaso Maria Ungetti</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>e657ffed-fda7-473f-b9dc-f943ec236f53</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Golden Circle</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>pseudonymph.com</t>
-        </is>
-      </c>
-      <c r="E13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>